<commit_message>
Twelfth  Commit Polidhing the GUI.
There's a problem when the program is restarted and the nodes.
Will have to look for it.
</commit_message>
<xml_diff>
--- a/out/production/COM212_FinalProject/seed/ExcelMovieSeed.xlsx
+++ b/out/production/COM212_FinalProject/seed/ExcelMovieSeed.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deringezgin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deringezgin/IdeaProjects/COM212_FinalProject/seed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11ACD473-041F-6A4D-ACF8-D517EEF5D2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3208C57-F01A-6141-BB04-7A648FDED824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" xr2:uid="{8EA1F4E6-B9FC-A845-BDFF-B091DA970467}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21120" xr2:uid="{8EA1F4E6-B9FC-A845-BDFF-B091DA970467}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -557,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668A88E2-6163-AD41-94BA-FD3FB38730D6}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScale="178" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,7 +568,7 @@
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -576,16 +576,13 @@
         <v>20010422</v>
       </c>
       <c r="C1">
-        <v>10000</v>
+        <v>88</v>
       </c>
       <c r="D1">
-        <v>88</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -593,16 +590,13 @@
         <v>20040519</v>
       </c>
       <c r="C2">
-        <v>10001</v>
+        <v>89</v>
       </c>
       <c r="D2">
-        <v>89</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -610,16 +604,13 @@
         <v>20070518</v>
       </c>
       <c r="C3">
-        <v>10002</v>
+        <v>42</v>
       </c>
       <c r="D3">
-        <v>42</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -627,16 +618,13 @@
         <v>20060609</v>
       </c>
       <c r="C4">
-        <v>10003</v>
+        <v>75</v>
       </c>
       <c r="D4">
-        <v>75</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -644,16 +632,13 @@
         <v>20110624</v>
       </c>
       <c r="C5">
-        <v>10004</v>
+        <v>39</v>
       </c>
       <c r="D5">
-        <v>39</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -661,16 +646,13 @@
         <v>20170616</v>
       </c>
       <c r="C6">
-        <v>10005</v>
+        <v>69</v>
       </c>
       <c r="D6">
-        <v>69</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -678,16 +660,13 @@
         <v>20130809</v>
       </c>
       <c r="C7">
-        <v>10006</v>
+        <v>26</v>
       </c>
       <c r="D7">
-        <v>26</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -695,16 +674,13 @@
         <v>20140718</v>
       </c>
       <c r="C8">
-        <v>10007</v>
+        <v>44</v>
       </c>
       <c r="D8">
-        <v>44</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -712,16 +688,13 @@
         <v>19720315</v>
       </c>
       <c r="C9">
-        <v>10008</v>
+        <v>97</v>
       </c>
       <c r="D9">
-        <v>97</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -729,16 +702,13 @@
         <v>19741220</v>
       </c>
       <c r="C10">
-        <v>10009</v>
+        <v>96</v>
       </c>
       <c r="D10">
-        <v>96</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -746,16 +716,13 @@
         <v>19901225</v>
       </c>
       <c r="C11">
-        <v>10010</v>
+        <v>66</v>
       </c>
       <c r="D11">
-        <v>66</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -763,16 +730,13 @@
         <v>19990519</v>
       </c>
       <c r="C12">
-        <v>10011</v>
+        <v>52</v>
       </c>
       <c r="D12">
-        <v>52</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -780,16 +744,13 @@
         <v>20020516</v>
       </c>
       <c r="C13">
-        <v>10012</v>
+        <v>65</v>
       </c>
       <c r="D13">
-        <v>65</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -797,16 +758,13 @@
         <v>20050519</v>
       </c>
       <c r="C14">
-        <v>10013</v>
+        <v>79</v>
       </c>
       <c r="D14">
-        <v>79</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -814,16 +772,13 @@
         <v>19770525</v>
       </c>
       <c r="C15">
-        <v>10014</v>
+        <v>93</v>
       </c>
       <c r="D15">
-        <v>93</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -831,16 +786,13 @@
         <v>19800521</v>
       </c>
       <c r="C16">
-        <v>10015</v>
+        <v>95</v>
       </c>
       <c r="D16">
-        <v>95</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -848,16 +800,13 @@
         <v>19830525</v>
       </c>
       <c r="C17">
-        <v>10016</v>
+        <v>83</v>
       </c>
       <c r="D17">
-        <v>83</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -865,16 +814,13 @@
         <v>20151218</v>
       </c>
       <c r="C18">
-        <v>10017</v>
+        <v>93</v>
       </c>
       <c r="D18">
-        <v>93</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -882,16 +828,13 @@
         <v>20171215</v>
       </c>
       <c r="C19">
-        <v>10018</v>
+        <v>91</v>
       </c>
       <c r="D19">
-        <v>91</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -899,16 +842,13 @@
         <v>20191220</v>
       </c>
       <c r="C20">
-        <v>10019</v>
+        <v>51</v>
       </c>
       <c r="D20">
-        <v>51</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -916,16 +856,13 @@
         <v>20161216</v>
       </c>
       <c r="C21">
-        <v>10020</v>
+        <v>84</v>
       </c>
       <c r="D21">
-        <v>84</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -933,16 +870,13 @@
         <v>20080518</v>
       </c>
       <c r="C22">
-        <v>10021</v>
+        <v>69</v>
       </c>
       <c r="D22">
-        <v>69</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -950,16 +884,13 @@
         <v>20080815</v>
       </c>
       <c r="C23">
-        <v>10022</v>
+        <v>19</v>
       </c>
       <c r="D23">
-        <v>19</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -967,16 +898,13 @@
         <v>19820625</v>
       </c>
       <c r="C24">
-        <v>10023</v>
+        <v>89</v>
       </c>
       <c r="D24">
-        <v>89</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -984,16 +912,13 @@
         <v>20171006</v>
       </c>
       <c r="C25">
-        <v>10024</v>
+        <v>88</v>
       </c>
       <c r="D25">
-        <v>88</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1001,16 +926,13 @@
         <v>20211022</v>
       </c>
       <c r="C26">
-        <v>10025</v>
+        <v>83</v>
       </c>
       <c r="D26">
-        <v>83</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1018,16 +940,13 @@
         <v>20240225</v>
       </c>
       <c r="C27">
-        <v>10026</v>
+        <v>93</v>
       </c>
       <c r="D27">
-        <v>93</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1035,16 +954,13 @@
         <v>20120712</v>
       </c>
       <c r="C28">
-        <v>10027</v>
+        <v>87</v>
       </c>
       <c r="D28">
-        <v>87</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1052,16 +968,13 @@
         <v>20020831</v>
       </c>
       <c r="C29">
-        <v>10028</v>
+        <v>96</v>
       </c>
       <c r="D29">
-        <v>96</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1069,16 +982,13 @@
         <v>19900713</v>
       </c>
       <c r="C30">
-        <v>10029</v>
+        <v>93</v>
       </c>
       <c r="D30">
-        <v>93</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1086,16 +996,13 @@
         <v>19910719</v>
       </c>
       <c r="C31">
-        <v>10030</v>
+        <v>96</v>
       </c>
       <c r="D31">
-        <v>96</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1103,16 +1010,13 @@
         <v>19951122</v>
       </c>
       <c r="C32">
-        <v>10031</v>
+        <v>100</v>
       </c>
       <c r="D32">
-        <v>100</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1120,16 +1024,13 @@
         <v>19991124</v>
       </c>
       <c r="C33">
-        <v>10032</v>
+        <v>100</v>
       </c>
       <c r="D33">
-        <v>100</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1137,16 +1038,13 @@
         <v>20100618</v>
       </c>
       <c r="C34">
-        <v>10033</v>
+        <v>98</v>
       </c>
       <c r="D34">
-        <v>98</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1154,16 +1052,13 @@
         <v>20190621</v>
       </c>
       <c r="C35">
-        <v>10034</v>
+        <v>97</v>
       </c>
       <c r="D35">
-        <v>97</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1171,16 +1066,13 @@
         <v>19990331</v>
       </c>
       <c r="C36">
-        <v>10035</v>
+        <v>83</v>
       </c>
       <c r="D36">
-        <v>83</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1188,16 +1080,13 @@
         <v>20030515</v>
       </c>
       <c r="C37">
-        <v>10036</v>
+        <v>74</v>
       </c>
       <c r="D37">
-        <v>74</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1205,16 +1094,13 @@
         <v>20031027</v>
       </c>
       <c r="C38">
-        <v>10037</v>
+        <v>34</v>
       </c>
       <c r="D38">
-        <v>34</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1222,16 +1108,13 @@
         <v>20211222</v>
       </c>
       <c r="C39">
-        <v>10038</v>
+        <v>63</v>
       </c>
       <c r="D39">
-        <v>63</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1239,16 +1122,13 @@
         <v>20190927</v>
       </c>
       <c r="C40">
-        <v>10039</v>
+        <v>95</v>
       </c>
       <c r="D40">
-        <v>95</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1256,16 +1136,13 @@
         <v>20230721</v>
       </c>
       <c r="C41">
-        <v>10040</v>
+        <v>93</v>
       </c>
       <c r="D41">
-        <v>93</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1273,16 +1150,13 @@
         <v>20230721</v>
       </c>
       <c r="C42">
-        <v>10041</v>
+        <v>88</v>
       </c>
       <c r="D42">
-        <v>88</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1290,16 +1164,13 @@
         <v>19981023</v>
       </c>
       <c r="C43">
-        <v>10042</v>
+        <v>81</v>
       </c>
       <c r="D43">
-        <v>81</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1307,16 +1178,13 @@
         <v>20180519</v>
       </c>
       <c r="C44">
-        <v>10043</v>
+        <v>31</v>
       </c>
       <c r="D44">
-        <v>31</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1324,16 +1192,13 @@
         <v>19940204</v>
       </c>
       <c r="C45">
-        <v>10044</v>
+        <v>98</v>
       </c>
       <c r="D45">
-        <v>98</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1341,16 +1206,13 @@
         <v>20030328</v>
       </c>
       <c r="C46">
-        <v>10045</v>
+        <v>95</v>
       </c>
       <c r="D46">
-        <v>95</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1358,16 +1220,13 @@
         <v>20180323</v>
       </c>
       <c r="C47">
-        <v>10046</v>
+        <v>90</v>
       </c>
       <c r="D47">
-        <v>90</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1375,16 +1234,13 @@
         <v>20091113</v>
       </c>
       <c r="C48">
-        <v>10047</v>
+        <v>93</v>
       </c>
       <c r="D48">
-        <v>93</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1392,16 +1248,13 @@
         <v>20150619</v>
       </c>
       <c r="C49">
-        <v>10048</v>
+        <v>98</v>
       </c>
       <c r="D49">
-        <v>98</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1409,16 +1262,13 @@
         <v>20240322</v>
       </c>
       <c r="C50">
-        <v>10049</v>
+        <v>91</v>
       </c>
       <c r="D50">
-        <v>91</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1426,16 +1276,13 @@
         <v>20011102</v>
       </c>
       <c r="C51">
-        <v>10050</v>
+        <v>96</v>
       </c>
       <c r="D51">
-        <v>96</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1443,16 +1290,13 @@
         <v>20070629</v>
       </c>
       <c r="C52">
-        <v>10051</v>
+        <v>96</v>
       </c>
       <c r="D52">
-        <v>96</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1460,16 +1304,13 @@
         <v>20080627</v>
       </c>
       <c r="C53">
-        <v>10052</v>
+        <v>95</v>
       </c>
       <c r="D53">
-        <v>95</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1477,16 +1318,13 @@
         <v>20240412</v>
       </c>
       <c r="C54">
-        <v>10053</v>
+        <v>95</v>
       </c>
       <c r="D54">
-        <v>95</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1494,12 +1332,9 @@
         <v>20090529</v>
       </c>
       <c r="C55">
-        <v>10054</v>
+        <v>98</v>
       </c>
       <c r="D55">
-        <v>98</v>
-      </c>
-      <c r="E55">
         <v>1</v>
       </c>
     </row>

</xml_diff>